<commit_message>
Updated Image upload size
</commit_message>
<xml_diff>
--- a/Migration/Employees/Input/Employees Profile - V2.xlsx
+++ b/Migration/Employees/Input/Employees Profile - V2.xlsx
@@ -1101,7 +1101,6 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1124,7 +1123,6 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1132,21 +1130,18 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1154,7 +1149,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1162,7 +1156,6 @@
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1170,7 +1163,6 @@
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -1178,21 +1170,19 @@
       <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="7"/>
-      <color rgb="FF222222"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1801,7 +1791,7 @@
     <cellStyle name="Pivot Table Value" xfId="26"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1870,13 +1860,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFF00"/>
           <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.7999"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3954,15 +3937,6 @@
   <dataFields count="1">
     <dataField name="Count of S.No" fld="0" subtotal="count" numFmtId="164"/>
   </dataFields>
-  <formats count="1">
-    <format dxfId="9">
-      <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="3" count="1"/>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
 </pivotTableDefinition>
 </file>
@@ -3972,9 +3946,10 @@
   <autoFilter ref="A11:AT43">
     <filterColumn colId="45">
       <filters>
-        <filter val="Accounting, Payment Document, Inquiry, Testing"/>
-        <filter val="Payment Document"/>
-        <filter val="Payment Document, Inquiry"/>
+        <filter val="Inspection"/>
+        <filter val="Inspection, Site Supervisor"/>
+        <filter val="Site Inspection"/>
+        <filter val="Site Inspection, Testing, Work allocation, Supervisor"/>
         <filter val="Site Inspection, Testing, Work allocation, Supervisor, Payment Document"/>
       </filters>
     </filterColumn>
@@ -4073,14 +4048,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -4088,67 +4063,25 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -4167,35 +4100,11 @@
           <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -4222,7 +4131,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.11"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -4244,7 +4153,7 @@
       <c r="F4" s="0"/>
       <c r="G4" s="0"/>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -4267,7 +4176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="s">
         <v>9</v>
       </c>
@@ -4290,7 +4199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
@@ -4303,7 +4212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
@@ -4326,7 +4235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
         <v>20</v>
       </c>
@@ -4339,7 +4248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
         <v>21</v>
       </c>
@@ -4362,7 +4271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
       <c r="C11" s="8" t="s">
@@ -4381,7 +4290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
         <v>28</v>
       </c>
@@ -4394,7 +4303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
         <v>29</v>
       </c>
@@ -4417,7 +4326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
       <c r="C14" s="8" t="s">
@@ -4436,7 +4345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
         <v>38</v>
       </c>
@@ -4449,7 +4358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
         <v>39</v>
       </c>
@@ -4472,7 +4381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
         <v>45</v>
       </c>
@@ -4485,7 +4394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
         <v>46</v>
       </c>
@@ -4508,7 +4417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="19"/>
       <c r="B19" s="8" t="s">
         <v>52</v>
@@ -4529,7 +4438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="19"/>
       <c r="B20" s="8" t="s">
         <v>56</v>
@@ -4550,7 +4459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="19"/>
       <c r="B21" s="8" t="s">
         <v>60</v>
@@ -4571,7 +4480,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19"/>
       <c r="B22" s="16" t="s">
         <v>63</v>
@@ -4592,7 +4501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19"/>
       <c r="B23" s="18"/>
       <c r="C23" s="8" t="s">
@@ -4611,7 +4520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="19"/>
       <c r="B24" s="8" t="s">
         <v>67</v>
@@ -4632,7 +4541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="19"/>
       <c r="B25" s="8" t="s">
         <v>70</v>
@@ -4653,7 +4562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19"/>
       <c r="B26" s="8" t="s">
         <v>74</v>
@@ -4674,7 +4583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="17"/>
       <c r="B27" s="8" t="s">
         <v>78</v>
@@ -4695,7 +4604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="11" t="s">
         <v>83</v>
       </c>
@@ -4708,7 +4617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="15" t="s">
         <v>10</v>
       </c>
@@ -4731,7 +4640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="19"/>
       <c r="B30" s="20"/>
       <c r="C30" s="8" t="s">
@@ -4750,7 +4659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="19"/>
       <c r="B31" s="20"/>
       <c r="C31" s="8" t="s">
@@ -4769,7 +4678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="19"/>
       <c r="B32" s="20"/>
       <c r="C32" s="8" t="s">
@@ -4788,7 +4697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="19"/>
       <c r="B33" s="20"/>
       <c r="C33" s="8" t="s">
@@ -4807,7 +4716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="19"/>
       <c r="B34" s="20"/>
       <c r="C34" s="8" t="s">
@@ -4826,7 +4735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="19"/>
       <c r="B35" s="20"/>
       <c r="C35" s="8" t="s">
@@ -4845,7 +4754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="19"/>
       <c r="B36" s="20"/>
       <c r="C36" s="16" t="s">
@@ -4864,7 +4773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="19"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -4881,7 +4790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="19"/>
       <c r="B38" s="16" t="s">
         <v>98</v>
@@ -4902,7 +4811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="17"/>
       <c r="B39" s="18"/>
       <c r="C39" s="8" t="s">
@@ -4921,7 +4830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="11" t="s">
         <v>103</v>
       </c>
@@ -4934,7 +4843,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="21" t="s">
         <v>104</v>
       </c>
@@ -4966,11 +4875,11 @@
   <dimension ref="A1:AT45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="112" zoomScaleNormal="112" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="11" topLeftCell="AS12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="11" topLeftCell="AQ21" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AS1" activeCellId="0" sqref="AS1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="B39" activeCellId="0" sqref="B39"/>
+      <selection pane="topRight" activeCell="AQ1" activeCellId="0" sqref="AQ1"/>
+      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="AT21" activeCellId="0" sqref="AT21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.78125" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
@@ -5067,7 +4976,7 @@
       <c r="AL1" s="28"/>
       <c r="AM1" s="28"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="29" t="s">
         <v>106</v>
       </c>
@@ -5110,7 +5019,7 @@
       <c r="AL2" s="28"/>
       <c r="AM2" s="28"/>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="29" t="s">
         <v>107</v>
       </c>
@@ -5153,7 +5062,7 @@
       <c r="AL3" s="28"/>
       <c r="AM3" s="28"/>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="29" t="s">
         <v>108</v>
       </c>
@@ -5196,7 +5105,7 @@
       <c r="AL4" s="28"/>
       <c r="AM4" s="28"/>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="29" t="s">
         <v>109</v>
       </c>
@@ -5239,7 +5148,7 @@
       <c r="AL5" s="28"/>
       <c r="AM5" s="28"/>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="30" t="s">
         <v>110</v>
       </c>
@@ -5325,7 +5234,7 @@
       <c r="AL7" s="28"/>
       <c r="AM7" s="28"/>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="29" t="s">
         <v>112</v>
       </c>
@@ -5368,7 +5277,7 @@
       <c r="AL8" s="28"/>
       <c r="AM8" s="28"/>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="32" t="s">
         <v>113</v>
       </c>
@@ -5411,7 +5320,7 @@
       <c r="AL9" s="28"/>
       <c r="AM9" s="28"/>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="33"/>
       <c r="B10" s="34"/>
       <c r="C10" s="35" t="s">
@@ -5698,7 +5607,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="46" t="n">
         <f aca="false">A12+1</f>
         <v>2</v>
@@ -5765,7 +5674,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="16.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="46" t="n">
         <f aca="false">A13+1</f>
         <v>3</v>
@@ -5858,7 +5767,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="46" t="n">
         <f aca="false">A14+1</f>
         <v>4</v>
@@ -6046,7 +5955,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="22.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="46" t="n">
         <f aca="false">A16+1</f>
         <v>6</v>
@@ -6139,7 +6048,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="46" t="n">
         <f aca="false">A17+1</f>
         <v>7</v>
@@ -6236,7 +6145,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="46" t="n">
         <f aca="false">A18+1</f>
         <v>8</v>
@@ -6337,7 +6246,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="46" t="n">
         <f aca="false">A19+1</f>
         <v>9</v>
@@ -6440,7 +6349,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="46" t="n">
         <f aca="false">A20+1</f>
         <v>10</v>
@@ -6543,7 +6452,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="46" t="n">
         <f aca="false">A21+1</f>
         <v>11</v>
@@ -6636,7 +6545,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="46" t="n">
         <f aca="false">A22+1</f>
         <v>12</v>
@@ -6945,7 +6854,7 @@
       <c r="AS25" s="53"/>
       <c r="AT25" s="63"/>
     </row>
-    <row r="26" customFormat="false" ht="16.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="46" t="n">
         <f aca="false">A25+1</f>
         <v>15</v>
@@ -7048,7 +6957,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="32.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="46" t="n">
         <f aca="false">A26+1</f>
         <v>16</v>
@@ -7139,7 +7048,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="32.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="46" t="n">
         <f aca="false">A27+1</f>
         <v>17</v>
@@ -7234,7 +7143,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="46" t="n">
         <f aca="false">A28+1</f>
         <v>18</v>
@@ -7489,7 +7398,7 @@
       <c r="AS31" s="53"/>
       <c r="AT31" s="63"/>
     </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="46" t="n">
         <f aca="false">A31+1</f>
         <v>21</v>
@@ -7661,7 +7570,7 @@
       <c r="AS33" s="53"/>
       <c r="AT33" s="63"/>
     </row>
-    <row r="34" customFormat="false" ht="22.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="46" t="n">
         <f aca="false">A33+1</f>
         <v>23</v>
@@ -7952,7 +7861,7 @@
       <c r="AS36" s="53"/>
       <c r="AT36" s="63"/>
     </row>
-    <row r="37" customFormat="false" ht="16.4" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="46" t="n">
         <f aca="false">A36+1</f>
         <v>26</v>
@@ -8023,7 +7932,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="22.35" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="46" t="n">
         <f aca="false">A37+1</f>
         <v>27</v>
@@ -8246,7 +8155,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="46" t="n">
         <f aca="false">A40+1</f>
         <v>30</v>
@@ -8309,7 +8218,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="46" t="n">
         <f aca="false">A41+1</f>
         <v>31</v>
@@ -8360,7 +8269,7 @@
       <c r="AS42" s="53"/>
       <c r="AT42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="46" t="n">
         <f aca="false">A42+1</f>
         <v>32</v>
@@ -8435,10 +8344,10 @@
       <c r="AS43" s="75"/>
       <c r="AT43" s="76"/>
     </row>
-    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="77"/>
     </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="77"/>
       <c r="AK45" s="78"/>
     </row>

</xml_diff>